<commit_message>
finished xlsx generation part now going to make it into a script
</commit_message>
<xml_diff>
--- a/temp/temp.xlsx
+++ b/temp/temp.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -418,19 +421,23 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="19.5" customWidth="1" style="1" min="1" max="1"/>
+    <col width="85" customWidth="1" style="2" min="2" max="2"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="65" customHeight="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Anshel1999</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -468,13 +475,13 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+    <row r="2" ht="65" customHeight="1">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Fine2011</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <r>
             <t>Aspects of Nonabelian Group Based Cryptography: A Survey and Open Problems / B. Fine [и др.] // arXiv.org, e-Print Archive Mathematics. — 2011. — DOI:</t>
@@ -494,13 +501,13 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="3" ht="65" customHeight="1">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Bezverkhnij1999</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -520,13 +527,13 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="4" ht="65" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Bezverkhniy2019</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -555,13 +562,13 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+    <row r="5" ht="65" customHeight="1">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Bigdely2013</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -581,13 +588,13 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+    <row r="6" ht="65" customHeight="1">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Bishop2020</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -616,13 +623,13 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+    <row r="7" ht="65" customHeight="1">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Blackburn2009</t>
         </is>
       </c>
-      <c r="B7" s="1" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -672,13 +679,13 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+    <row r="8" ht="65" customHeight="1">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Coulon2013</t>
         </is>
       </c>
-      <c r="B8" s="1" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -704,13 +711,13 @@
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+    <row r="9" ht="65" customHeight="1">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Coulon2019</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -739,13 +746,13 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+    <row r="10" ht="65" customHeight="1">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Flores2016</t>
         </is>
       </c>
-      <c r="B10" s="1" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -780,13 +787,13 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+    <row r="11" ht="65" customHeight="1">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Gromov1987</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -800,13 +807,13 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+    <row r="12" ht="65" customHeight="1">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Gruber2014</t>
         </is>
       </c>
-      <c r="B12" s="1" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -826,13 +833,13 @@
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+    <row r="13" ht="65" customHeight="1">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Habeeb2012</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -876,13 +883,13 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+    <row r="14" ht="65" customHeight="1">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Hasapis2015</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -920,13 +927,13 @@
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+    <row r="15" ht="65" customHeight="1">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Hull2016</t>
         </is>
       </c>
-      <c r="B15" s="1" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -952,13 +959,13 @@
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+    <row r="16" ht="65" customHeight="1">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Kalkan2014</t>
         </is>
       </c>
-      <c r="B16" s="1" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -972,13 +979,13 @@
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+    <row r="17" ht="65" customHeight="1">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Lee2020</t>
         </is>
       </c>
-      <c r="B17" s="1" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1022,13 +1029,13 @@
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+    <row r="18" ht="65" customHeight="1">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Myasnikov2008</t>
         </is>
       </c>
-      <c r="B18" s="1" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1072,13 +1079,13 @@
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+    <row r="19" ht="65" customHeight="1">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Shpilrain2018</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1104,13 +1111,13 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+    <row r="20" ht="65" customHeight="1">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Shpilrain2004</t>
         </is>
       </c>
-      <c r="B20" s="1" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1145,13 +1152,13 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+    <row r="21" ht="65" customHeight="1">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Shpilrain2006</t>
         </is>
       </c>
-      <c r="B21" s="1" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1186,13 +1193,13 @@
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+    <row r="22" ht="65" customHeight="1">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Безверхний1994</t>
         </is>
       </c>
-      <c r="B22" s="1" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1206,13 +1213,13 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
+    <row r="23" ht="65" customHeight="1">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Безверхний2014</t>
         </is>
       </c>
-      <c r="B23" s="1" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1226,13 +1233,13 @@
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+    <row r="24" ht="65" customHeight="1">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Безверхний2010</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1246,13 +1253,13 @@
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+    <row r="25" ht="65" customHeight="1">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Линдон1980</t>
         </is>
       </c>
-      <c r="B25" s="1" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1275,13 +1282,13 @@
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+    <row r="26" ht="65" customHeight="1">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Магнус1974</t>
         </is>
       </c>
-      <c r="B26" s="1" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1313,13 +1320,13 @@
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+    <row r="27" ht="65" customHeight="1">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Ольшанский1989</t>
         </is>
       </c>
-      <c r="B27" s="1" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1335,6 +1342,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="1" fitToWidth="1"/>
 </worksheet>
 </file>
</xml_diff>